<commit_message>
221122 suhwa new crawling_ing
</commit_message>
<xml_diff>
--- a/관련 문서/일자별 진행상황.xlsx
+++ b/관련 문서/일자별 진행상황.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSAFY\ssafy_workspace\Where_Is_My_House\관련 문서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSAFY\workspace\Where_Is_My_House\관련 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE1B6B5-C6B7-46EC-B357-9FB85255C29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34755" yWindow="810" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34755" yWindow="810" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>희진</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,15 +121,48 @@
 에러파티랄까</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>관심지역
+병원
+코로나 진료소
+지도 뿌리기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상권정보
+유지보수
+뉴스 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관심지역, 상권정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상권정보 마무리
+뉴스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유지보수
+ui 바꾸기
+그래프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 마무리
+ui 바꾸기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -216,6 +248,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -503,27 +541,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="10.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="26.125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.5" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="14.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="10" customWidth="1"/>
+    <col min="8" max="8" width="40.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
+    <row r="1" spans="1:8">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="2">
         <v>44882</v>
       </c>
@@ -539,9 +579,12 @@
       <c r="G1" s="2">
         <v>44888</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="H1" s="2">
+        <v>44889</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="37.5" customHeight="1">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -553,14 +596,19 @@
       <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="11" t="s">
+      <c r="E2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:8" ht="24">
+      <c r="A3" s="12"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -570,10 +618,11 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" ht="24">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -585,12 +634,17 @@
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
+      <c r="H4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" ht="48">
+      <c r="A5" s="12"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -600,17 +654,22 @@
       <c r="D5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" ht="24">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -623,13 +682,13 @@
       <c r="D8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" ht="36">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -645,8 +704,9 @@
         <v>14</v>
       </c>
       <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -657,7 +717,7 @@
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="G2:G9"/>
+    <mergeCell ref="H2:H9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>